<commit_message>
Latest version including inattention monitoring taxonomy
</commit_message>
<xml_diff>
--- a/literature_review/project_plan.xlsx
+++ b/literature_review/project_plan.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmssmith/MSc/Thesis/literature_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBB9C66-E794-D04D-906B-B66E16B58BEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A723670A-BA1C-F04C-9623-46C5C49B22E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37540" yWindow="6500" windowWidth="31520" windowHeight="16120" activeTab="2" xr2:uid="{42E1EFD9-6BFF-B54C-A3AF-2A11D6F807B3}"/>
+    <workbookView xWindow="38980" yWindow="4160" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{42E1EFD9-6BFF-B54C-A3AF-2A11D6F807B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Thesis plan" sheetId="2" r:id="rId2"/>
-    <sheet name="Summary" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Summary graph" sheetId="4" r:id="rId5"/>
+    <sheet name="radar_frequencies" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Thesis plan" sheetId="2" r:id="rId3"/>
+    <sheet name="Summary" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Summary graph" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>TOTAL</t>
   </si>
@@ -47,9 +48,6 @@
   </si>
   <si>
     <t>Percentage</t>
-  </si>
-  <si>
-    <t>Cumulative frequency</t>
   </si>
   <si>
     <t>Item</t>
@@ -86,9 +84,6 @@
   </si>
   <si>
     <t>Final report Submission</t>
-  </si>
-  <si>
-    <t>Final report draft complete</t>
   </si>
   <si>
     <t>Final report structure agreed</t>
@@ -234,6 +229,21 @@
   <si>
     <t>Combined</t>
   </si>
+  <si>
+    <t>Cumulative percentage</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Report writing</t>
+  </si>
+  <si>
+    <t>Report draft review</t>
+  </si>
+  <si>
+    <t>Experiment set up complete</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +291,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -760,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -913,6 +935,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,6 +957,519 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Usage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of different radar freqencies for vital sign detection</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD79-004A-8407-55DB140E0C53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="122983680"/>
+        <c:axId val="123255712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="122983680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radar frequency (GHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="123255712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="123255712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percenetage of considered</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> works</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="122983680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -990,7 +1528,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cumulative frequency</c:v>
+                  <c:v>Cumulative percentage</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1334,7 +1872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1734,7 +2272,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1794,7 +2332,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cumulative frequency</c:v>
+                  <c:v>Cumulative percentage</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2003,6 +2541,7 @@
         <c:axId val="100968848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2107,7 +2646,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3125,8 +3664,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3153,8 +3732,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3255,7 +3834,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3287,10 +3866,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3330,23 +3909,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3451,8 +4029,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3584,20 +4162,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3611,17 +4188,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4158,7 +4724,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4185,8 +4751,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4287,7 +4853,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4319,10 +4885,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4362,22 +4928,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4482,8 +5049,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4615,19 +5182,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4641,6 +5209,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5163,11 +5742,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1D29BF80-B476-DD4E-8ACB-FA32738E5071}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E44E16C1-190A-0F47-9BB9-43774AF699A7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="153" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5175,6 +6268,39 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9313333" cy="6076078"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CADE9153-3A91-464A-AD2F-9E7608AF0398}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5214,16 +6340,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5250,16 +6376,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5287,7 +6413,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -5619,8 +6745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2E0377-B633-7E48-A58A-008AFD0AF079}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5636,7 +6762,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -5860,10 +6986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23B3462-3B3E-8745-96B8-DDECE4A69225}">
-  <dimension ref="B2:V22"/>
+  <dimension ref="B2:V25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5876,7 +7002,7 @@
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4">
         <v>44449</v>
@@ -5884,7 +7010,7 @@
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>44447</v>
@@ -5892,41 +7018,41 @@
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
       <c r="V8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7">
         <v>44319</v>
@@ -5988,7 +7114,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>18</v>
@@ -6050,10 +7176,10 @@
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -6063,74 +7189,136 @@
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>23</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
       <c r="C15" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
-      <c r="C16" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="60"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="60"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
+      <c r="C17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="N19" s="58"/>
+      <c r="R19" s="58"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>16</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="O20" s="58"/>
+      <c r="S20" s="58"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="V21" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="S21" s="59"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="V22" s="10"/>
+        <v>65</v>
+      </c>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B23" s="8"/>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="8"/>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="V25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B11:B22"/>
+    <mergeCell ref="B11:B25"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="M8:P8"/>
@@ -6144,8 +7332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759C579E-4770-9340-9F04-E0C47877620A}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6163,21 +7351,21 @@
     <row r="2" spans="1:21" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
       <c r="E2" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
       <c r="J2" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K2" s="41"/>
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
       <c r="N2" s="42"/>
       <c r="O2" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
@@ -6189,64 +7377,64 @@
     <row r="3" spans="1:21" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="F3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="K3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="L3" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="14" t="s">
+      <c r="R3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="U3" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -6254,7 +7442,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="18">
         <v>1</v>
@@ -6293,7 +7481,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="19">
         <v>1</v>
@@ -6328,7 +7516,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="19">
         <v>1</v>
@@ -6361,7 +7549,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
@@ -6392,7 +7580,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="24">
@@ -6427,7 +7615,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="24">
@@ -6458,7 +7646,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="24">
@@ -6489,7 +7677,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="24">
@@ -6520,7 +7708,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="24">
@@ -6551,7 +7739,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="24">
@@ -6582,7 +7770,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="24">
@@ -6617,7 +7805,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="24">
@@ -6656,7 +7844,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="19">
         <v>1</v>
@@ -6701,7 +7889,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="20">
         <v>1</v>
@@ -6736,7 +7924,7 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="30">
         <f>SUM(C4:C17)</f>
@@ -6817,7 +8005,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B19" s="31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E19" s="35">
         <f>SUM(E4:E7)</f>
@@ -6890,7 +8078,7 @@
     </row>
     <row r="20" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="37">
         <f>SUM(E8:E15)</f>
@@ -6964,21 +8152,21 @@
     <row r="21" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C22" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="41"/>
       <c r="G22" s="42"/>
       <c r="H22" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
       <c r="L22" s="42"/>
       <c r="M22" s="40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N22" s="41"/>
       <c r="O22" s="41"/>
@@ -6989,60 +8177,60 @@
     </row>
     <row r="23" spans="1:21" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="50" t="s">
-        <v>31</v>
-      </c>
       <c r="J23" s="50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K23" s="50" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L23" s="51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M23" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="N23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="O23" s="50" t="s">
+      <c r="P23" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q23" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="R23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="P23" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q23" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="R23" s="50" t="s">
-        <v>40</v>
-      </c>
       <c r="S23" s="51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="46">
         <f>E19</f>
@@ -7115,7 +8303,7 @@
     </row>
     <row r="25" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="56" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="20">
         <f>E20</f>
@@ -7188,7 +8376,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26">
         <f>SUM(E16:E17)</f>
@@ -7288,71 +8476,71 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
-      </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7408,7 +8596,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7464,7 +8652,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>1</v>

</xml_diff>